<commit_message>
SE RENOMBRO ACTIVITY ADDFRIEND
El nuevo nombre es AddFriendActivity y se modificaron todas las ocurrencias del nombre anterior para que tuvieran el nuevo nombre
</commit_message>
<xml_diff>
--- a/Documentacion/MODELO-RELACIONAL.xlsx
+++ b/Documentacion/MODELO-RELACIONAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\OneDrive\Documentos\9no_semestre\APPS_DEV\proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\OneDrive\Documentos\9no_semestre\APPS_DEV\proyecto\apps-development-2020\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17301988-90C9-4DAA-A590-BB2901321DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FACDBC2-8877-4C6B-BA8E-1760779DACA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1E911CEC-BB13-4908-9602-AFC3D1ADC676}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>nombre</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>contraseña</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>apellidos</t>
+  </si>
+  <si>
+    <t>usuario</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,19 +484,19 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -504,7 +504,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -512,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -520,15 +520,15 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -544,29 +544,29 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
         <v>1</v>
@@ -574,18 +574,18 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>